<commit_message>
Finalized Yield, Price, Area data
</commit_message>
<xml_diff>
--- a/ABMdev/Data/NASS_Data/ID_yield_area_val_processing.xlsx
+++ b/ABMdev/Data/NASS_Data/ID_yield_area_val_processing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kek25/Documents/GitRepos/IM3-BoiseState/ABMdev/Data/NASS_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendrakaiser/Documents/GitRepos/IM3-BoiseState/ABMdev/Data/NASS_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A518797-5F3E-E844-A463-8FD0F749033E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14540" yWindow="3060" windowWidth="35560" windowHeight="24460" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11120" yWindow="10260" windowWidth="35560" windowHeight="16860" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="2010" sheetId="5" r:id="rId5"/>
     <sheet name="2015" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="166">
   <si>
     <t>Data Processing Notes</t>
   </si>
@@ -501,12 +500,45 @@
   </si>
   <si>
     <t>yield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAY, (EXCL ALFALFA) </t>
+  </si>
+  <si>
+    <t>(EXCL ALFALFA)</t>
+  </si>
+  <si>
+    <t>HAY</t>
+  </si>
+  <si>
+    <t>CORN</t>
+  </si>
+  <si>
+    <t>PRICE RECEIVED, MEASURED IN $ / BU</t>
+  </si>
+  <si>
+    <t>YIELD, MEASURED IN BU / ACRE</t>
+  </si>
+  <si>
+    <t>OATS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAY &amp; HAYLAGE, (EXCL ALFALFA) </t>
+  </si>
+  <si>
+    <t>HAY &amp; HAYLAGE</t>
+  </si>
+  <si>
+    <t>YIELD, MEASURED IN TONS / ACRE, DRY BASIS</t>
+  </si>
+  <si>
+    <t>TONS / ACRE, DRY BASIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -864,7 +896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1049,7 +1081,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:A36">
+  <sortState ref="A12:A36">
     <sortCondition ref="A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1057,7 +1089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1665,7 +1697,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
@@ -2378,15 +2410,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="41.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -3353,11 +3386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3867,7 +3900,7 @@
         <v>1600</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F23:F30" si="6">(C4*H4)+(D4*I4)+(E4*J4)</f>
+        <f t="shared" ref="F24:F30" si="6">(C4*H4)+(D4*I4)+(E4*J4)</f>
         <v>46697.303921568629</v>
       </c>
       <c r="G24">
@@ -4534,6 +4567,93 @@
       <c r="G74" s="3">
         <f>G73*30*30*0.000247105</f>
         <v>3372.8349870000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76">
+        <v>2010</v>
+      </c>
+      <c r="C76" t="s">
+        <v>155</v>
+      </c>
+      <c r="D76" t="s">
+        <v>145</v>
+      </c>
+      <c r="E76" t="s">
+        <v>156</v>
+      </c>
+      <c r="F76" t="s">
+        <v>111</v>
+      </c>
+      <c r="G76" t="s">
+        <v>147</v>
+      </c>
+      <c r="H76" t="s">
+        <v>157</v>
+      </c>
+      <c r="I76">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77">
+        <v>2010</v>
+      </c>
+      <c r="C77" t="s">
+        <v>155</v>
+      </c>
+      <c r="D77" t="s">
+        <v>115</v>
+      </c>
+      <c r="E77" t="s">
+        <v>156</v>
+      </c>
+      <c r="F77" t="s">
+        <v>111</v>
+      </c>
+      <c r="G77" t="s">
+        <v>29</v>
+      </c>
+      <c r="H77" t="s">
+        <v>157</v>
+      </c>
+      <c r="I77">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78">
+        <v>2010</v>
+      </c>
+      <c r="C78" t="s">
+        <v>155</v>
+      </c>
+      <c r="D78" t="s">
+        <v>119</v>
+      </c>
+      <c r="E78" t="s">
+        <v>156</v>
+      </c>
+      <c r="F78" t="s">
+        <v>111</v>
+      </c>
+      <c r="G78" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" t="s">
+        <v>157</v>
+      </c>
+      <c r="I78">
+        <v>2.1</v>
       </c>
     </row>
   </sheetData>
@@ -4542,11 +4662,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:S46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5486,6 +5606,358 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>174</v>
+      </c>
+      <c r="C48" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48">
+        <v>2015</v>
+      </c>
+      <c r="E48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>145</v>
+      </c>
+      <c r="G48" t="s">
+        <v>110</v>
+      </c>
+      <c r="H48" t="s">
+        <v>111</v>
+      </c>
+      <c r="I48" t="s">
+        <v>147</v>
+      </c>
+      <c r="J48" t="s">
+        <v>158</v>
+      </c>
+      <c r="K48">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>175</v>
+      </c>
+      <c r="C49" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49">
+        <v>2015</v>
+      </c>
+      <c r="E49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49" t="s">
+        <v>159</v>
+      </c>
+      <c r="G49" t="s">
+        <v>110</v>
+      </c>
+      <c r="H49" t="s">
+        <v>111</v>
+      </c>
+      <c r="I49" t="s">
+        <v>25</v>
+      </c>
+      <c r="J49" t="s">
+        <v>158</v>
+      </c>
+      <c r="K49">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>176</v>
+      </c>
+      <c r="C50" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50">
+        <v>2015</v>
+      </c>
+      <c r="E50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" t="s">
+        <v>160</v>
+      </c>
+      <c r="G50" t="s">
+        <v>110</v>
+      </c>
+      <c r="H50" t="s">
+        <v>111</v>
+      </c>
+      <c r="I50" t="s">
+        <v>94</v>
+      </c>
+      <c r="J50" t="s">
+        <v>158</v>
+      </c>
+      <c r="K50">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>177</v>
+      </c>
+      <c r="C51" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51">
+        <v>2015</v>
+      </c>
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
+        <v>145</v>
+      </c>
+      <c r="G51" t="s">
+        <v>110</v>
+      </c>
+      <c r="H51" t="s">
+        <v>111</v>
+      </c>
+      <c r="I51" t="s">
+        <v>147</v>
+      </c>
+      <c r="J51" t="s">
+        <v>158</v>
+      </c>
+      <c r="K51">
+        <v>205000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>178</v>
+      </c>
+      <c r="C52" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52">
+        <v>2015</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" t="s">
+        <v>119</v>
+      </c>
+      <c r="G52" t="s">
+        <v>110</v>
+      </c>
+      <c r="H52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I52" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" t="s">
+        <v>158</v>
+      </c>
+      <c r="K52">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>247</v>
+      </c>
+      <c r="C53" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53">
+        <v>2015</v>
+      </c>
+      <c r="E53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" t="s">
+        <v>145</v>
+      </c>
+      <c r="G53" t="s">
+        <v>110</v>
+      </c>
+      <c r="H53" t="s">
+        <v>111</v>
+      </c>
+      <c r="I53" t="s">
+        <v>147</v>
+      </c>
+      <c r="J53" t="s">
+        <v>161</v>
+      </c>
+      <c r="K53">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>248</v>
+      </c>
+      <c r="C54" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54">
+        <v>2015</v>
+      </c>
+      <c r="E54" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>159</v>
+      </c>
+      <c r="G54" t="s">
+        <v>110</v>
+      </c>
+      <c r="H54" t="s">
+        <v>111</v>
+      </c>
+      <c r="I54" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" t="s">
+        <v>161</v>
+      </c>
+      <c r="K54">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>249</v>
+      </c>
+      <c r="C55" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55">
+        <v>2015</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>160</v>
+      </c>
+      <c r="G55" t="s">
+        <v>110</v>
+      </c>
+      <c r="H55" t="s">
+        <v>111</v>
+      </c>
+      <c r="I55" t="s">
+        <v>94</v>
+      </c>
+      <c r="J55" t="s">
+        <v>161</v>
+      </c>
+      <c r="K55">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>197</v>
+      </c>
+      <c r="C56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56">
+        <v>2015</v>
+      </c>
+      <c r="E56" t="s">
+        <v>162</v>
+      </c>
+      <c r="F56" t="s">
+        <v>145</v>
+      </c>
+      <c r="G56" t="s">
+        <v>156</v>
+      </c>
+      <c r="H56" t="s">
+        <v>111</v>
+      </c>
+      <c r="I56" t="s">
+        <v>147</v>
+      </c>
+      <c r="J56" t="s">
+        <v>163</v>
+      </c>
+      <c r="K56">
+        <v>370000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>198</v>
+      </c>
+      <c r="C57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57">
+        <v>2015</v>
+      </c>
+      <c r="E57" t="s">
+        <v>162</v>
+      </c>
+      <c r="F57" t="s">
+        <v>164</v>
+      </c>
+      <c r="G57" t="s">
+        <v>156</v>
+      </c>
+      <c r="H57" t="s">
+        <v>111</v>
+      </c>
+      <c r="I57" t="s">
+        <v>165</v>
+      </c>
+      <c r="J57" t="s">
+        <v>163</v>
+      </c>
+      <c r="K57">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>181</v>
+      </c>
+      <c r="C58" t="s">
+        <v>152</v>
+      </c>
+      <c r="D58">
+        <v>2015</v>
+      </c>
+      <c r="E58" t="s">
+        <v>155</v>
+      </c>
+      <c r="F58" t="s">
+        <v>115</v>
+      </c>
+      <c r="G58" t="s">
+        <v>156</v>
+      </c>
+      <c r="H58" t="s">
+        <v>111</v>
+      </c>
+      <c r="I58" t="s">
+        <v>29</v>
+      </c>
+      <c r="J58" t="s">
+        <v>157</v>
+      </c>
+      <c r="K58">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>